<commit_message>
update integration get booking list
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/user/Login.xlsx
+++ b/src/main/resources/input_excel_file/user/Login.xlsx
@@ -48,7 +48,7 @@
     <t>expected_validation_data</t>
   </si>
   <si>
-    <t>TC_0001</t>
+    <t>TC_LOGIN_0001</t>
   </si>
   <si>
     <t>Verify Login Success</t>
@@ -69,7 +69,7 @@
 }</t>
   </si>
   <si>
-    <t>TC_0002</t>
+    <t>TC_LOGIN_0002</t>
   </si>
   <si>
     <t>Verify Login Wrong Username</t>
@@ -84,7 +84,7 @@
     <t>{"status_code": 500}</t>
   </si>
   <si>
-    <t>TC_0003</t>
+    <t>TC_LOGIN_0003</t>
   </si>
   <si>
     <t>Verify Login Wrong Password</t>
@@ -96,7 +96,7 @@
     <t>{"status_code": 400}</t>
   </si>
   <si>
-    <t>TC_0004</t>
+    <t>TC_LOGIN_0004</t>
   </si>
   <si>
     <t>Verify Login Wrong Username And Password</t>
@@ -131,10 +131,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -697,16 +697,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1400,11 +1400,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
+    <col min="1" max="1" width="17.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="21.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="14.8571428571429" customWidth="1"/>

</xml_diff>

<commit_message>
update create booking - login - report
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/user/Login.xlsx
+++ b/src/main/resources/input_excel_file/user/Login.xlsx
@@ -872,7 +872,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1400,7 +1400,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
update create booking member
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/user/Login.xlsx
+++ b/src/main/resources/input_excel_file/user/Login.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13080" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
-    <sheet name="testcase_v1" sheetId="1" r:id="rId1"/>
-    <sheet name="testcase_v2" sheetId="2" r:id="rId2"/>
+    <sheet name="testcase" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>tc_id</t>
   </si>
@@ -39,6 +38,9 @@
     <t>expected_result</t>
   </si>
   <si>
+    <t>input_placeholders</t>
+  </si>
+  <si>
     <t>user_name</t>
   </si>
   <si>
@@ -48,6 +50,21 @@
     <t>expected_validation_data</t>
   </si>
   <si>
+    <t>status_code</t>
+  </si>
+  <si>
+    <t>assert_token</t>
+  </si>
+  <si>
+    <t>assert_data.user_name</t>
+  </si>
+  <si>
+    <t>assert_data.partner_uid</t>
+  </si>
+  <si>
+    <t>assert_data.course_uid</t>
+  </si>
+  <si>
     <t>TC_LOGIN_0001</t>
   </si>
   <si>
@@ -57,88 +74,31 @@
     <t>success</t>
   </si>
   <si>
-    <t>phuongtt-chilinh</t>
-  </si>
-  <si>
-    <t>4aNefZgJHLO83Qc30N5Bjg==</t>
-  </si>
-  <si>
-    <t>{
-  "token": "NOT_NULL",
-  "data.user_name": "phuongtt-chilinh"
-}</t>
+    <t>login_request.json</t>
+  </si>
+  <si>
+    <t>phuongtt-auto-stg-01</t>
+  </si>
+  <si>
+    <t>PhuongTT@12345</t>
+  </si>
+  <si>
+    <t>login_expect.json</t>
+  </si>
+  <si>
+    <t>NOT_NULL</t>
+  </si>
+  <si>
+    <t>CHI-LINH</t>
+  </si>
+  <si>
+    <t>CHI-LINH-123</t>
   </si>
   <si>
     <t>TC_LOGIN_0002</t>
   </si>
   <si>
-    <t>Verify Login Wrong Username</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>saiuser</t>
-  </si>
-  <si>
-    <t>{"status_code": 500}</t>
-  </si>
-  <si>
-    <t>TC_LOGIN_0003</t>
-  </si>
-  <si>
-    <t>Verify Login Wrong Password</t>
-  </si>
-  <si>
-    <t>saimatkhau</t>
-  </si>
-  <si>
-    <t>{"status_code": 400}</t>
-  </si>
-  <si>
-    <t>TC_LOGIN_0004</t>
-  </si>
-  <si>
-    <t>Verify Login Wrong Username And Password</t>
-  </si>
-  <si>
-    <t>input_placeholders</t>
-  </si>
-  <si>
-    <t>status_code</t>
-  </si>
-  <si>
-    <t>assert_token</t>
-  </si>
-  <si>
-    <t>assert_data.user_name</t>
-  </si>
-  <si>
-    <t>assert_data.partner_uid</t>
-  </si>
-  <si>
-    <t>assert_data.course_uid</t>
-  </si>
-  <si>
-    <t>login_request.json</t>
-  </si>
-  <si>
-    <t>login_expect.json</t>
-  </si>
-  <si>
-    <t>NOT_NULL</t>
-  </si>
-  <si>
-    <t>CHI-LINH</t>
-  </si>
-  <si>
-    <t>CHI-LINH-01</t>
-  </si>
-  <si>
-    <t>Verify Login Success 01</t>
-  </si>
-  <si>
-    <t>phuongtt-chilinh01</t>
+    <t>Verify Login Success 02</t>
   </si>
 </sst>
 </file>
@@ -146,10 +106,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -179,19 +139,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -537,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -557,81 +517,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -741,25 +626,25 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -771,34 +656,34 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -883,54 +768,39 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -940,7 +810,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1465,268 +1335,148 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="17.2890625" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="21.859375" customWidth="1"/>
-    <col min="4" max="4" width="14.859375" customWidth="1"/>
-    <col min="5" max="5" width="19.859375" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="27" customHeight="1" spans="1:6">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" ht="58.75" spans="1:6">
-      <c r="A2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" ht="29" customHeight="1" spans="1:6">
-      <c r="A3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" ht="18.75" spans="1:6">
-      <c r="A4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" ht="35" customHeight="1" spans="1:6">
-      <c r="A5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="12.8828125" customWidth="1"/>
-    <col min="2" max="2" width="23.953125" customWidth="1"/>
-    <col min="3" max="3" width="21.859375" customWidth="1"/>
-    <col min="4" max="4" width="26.421875" customWidth="1"/>
-    <col min="5" max="5" width="14.859375" customWidth="1"/>
-    <col min="6" max="6" width="19.859375" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.96875" customWidth="1"/>
-    <col min="9" max="9" width="14.5859375" customWidth="1"/>
-    <col min="10" max="10" width="21.4765625" customWidth="1"/>
-    <col min="11" max="11" width="21.2421875" customWidth="1"/>
-    <col min="12" max="12" width="22.0625" customWidth="1"/>
+    <col min="1" max="1" width="12.8857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.952380952381" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.8571428571429" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.4190476190476" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.9428571428571" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6095238095238" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1619047619048" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.9714285714286" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5904761904762" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.4761904761905" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.2380952380952" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.0666666666667" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27" customHeight="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="31.5" spans="1:12">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7">
+        <v>200</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" ht="31.5" spans="1:12">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" ht="36" spans="1:12">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="7">
         <v>200</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" ht="41" customHeight="1" spans="1:12">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="3">
-        <v>200</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>33</v>
+      <c r="I3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="PhuongTT@12345"/>
+    <hyperlink ref="F3" r:id="rId1" display="PhuongTT@12345"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>